<commit_message>
Modify: fix some issues.
</commit_message>
<xml_diff>
--- a/storage/app/iprs/1/iprs.xlsx
+++ b/storage/app/iprs/1/iprs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Smoku\Pfron\pfron-backend\storage\app\iprs\1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91FB621B-BF21-4A16-AB8C-AC8A55C606DE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B160D71-5400-457F-9A00-D1D1E8552C4B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t>id</t>
   </si>
@@ -182,6 +182,12 @@
   </si>
   <si>
     <t>M1-W022</t>
+  </si>
+  <si>
+    <t>M1-W053</t>
+  </si>
+  <si>
+    <t>M1-W055</t>
   </si>
 </sst>
 </file>
@@ -2593,21 +2599,22 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U129"/>
+  <dimension ref="A1:AD130"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="O29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A57" sqref="A57:A99"/>
+      <selection pane="bottomRight" activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="10.625" style="14" customWidth="1"/>
+    <col min="25" max="25" width="12.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="15" customHeight="1" thickBot="1">
+    <row r="1" spans="1:30" ht="15" customHeight="1" thickBot="1">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -2657,22 +2664,49 @@
         <v>26</v>
       </c>
       <c r="Q1" s="2">
+        <v>27</v>
+      </c>
+      <c r="R1" s="2">
+        <v>28</v>
+      </c>
+      <c r="S1" s="2">
+        <v>29</v>
+      </c>
+      <c r="T1" s="2">
         <v>30</v>
       </c>
-      <c r="R1" s="2">
+      <c r="U1" s="2">
         <v>31</v>
       </c>
-      <c r="S1" s="2">
+      <c r="V1" s="2">
         <v>32</v>
       </c>
-      <c r="T1" s="2">
+      <c r="W1" s="2">
         <v>33</v>
       </c>
-      <c r="U1" s="2">
+      <c r="X1" s="2">
         <v>34</v>
       </c>
-    </row>
-    <row r="2" spans="1:21" ht="15" customHeight="1" thickBot="1">
+      <c r="Y1" s="2">
+        <v>35</v>
+      </c>
+      <c r="Z1" s="2">
+        <v>36</v>
+      </c>
+      <c r="AA1" s="2">
+        <v>37</v>
+      </c>
+      <c r="AB1" s="2">
+        <v>38</v>
+      </c>
+      <c r="AC1" s="2">
+        <v>39</v>
+      </c>
+      <c r="AD1" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30" ht="15" customHeight="1" thickBot="1">
       <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
@@ -2722,20 +2756,47 @@
         <v>4</v>
       </c>
       <c r="Q2" s="3">
+        <v>0</v>
+      </c>
+      <c r="R2" s="3">
+        <v>0</v>
+      </c>
+      <c r="S2" s="3">
+        <v>0</v>
+      </c>
+      <c r="T2" s="3">
         <v>96</v>
       </c>
-      <c r="R2" s="1">
+      <c r="U2" s="1">
         <v>52</v>
       </c>
-      <c r="S2" s="3">
+      <c r="V2" s="3">
         <v>2.5</v>
       </c>
-      <c r="T2" s="3">
+      <c r="W2" s="3">
         <v>11</v>
       </c>
-      <c r="U2" s="7"/>
-    </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1" thickBot="1">
+      <c r="X2" s="7"/>
+      <c r="Y2" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA2" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB2" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC2" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD2" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" ht="15" customHeight="1" thickBot="1">
       <c r="A3" s="11" t="s">
         <v>2</v>
       </c>
@@ -2785,20 +2846,47 @@
         <v>4</v>
       </c>
       <c r="Q3" s="3">
+        <v>0</v>
+      </c>
+      <c r="R3" s="3">
+        <v>0</v>
+      </c>
+      <c r="S3" s="3">
+        <v>0</v>
+      </c>
+      <c r="T3" s="3">
         <v>94.5</v>
       </c>
-      <c r="R3" s="3">
+      <c r="U3" s="3">
         <v>61</v>
       </c>
-      <c r="S3" s="3">
+      <c r="V3" s="3">
         <v>2</v>
       </c>
-      <c r="T3" s="3">
+      <c r="W3" s="3">
         <v>1</v>
       </c>
-      <c r="U3" s="7"/>
-    </row>
-    <row r="4" spans="1:21" ht="15" customHeight="1" thickBot="1">
+      <c r="X3" s="7"/>
+      <c r="Y3" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC3" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD3" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" ht="15" customHeight="1" thickBot="1">
       <c r="A4" s="11" t="s">
         <v>3</v>
       </c>
@@ -2848,20 +2936,47 @@
         <v>4</v>
       </c>
       <c r="Q4" s="3">
+        <v>0</v>
+      </c>
+      <c r="R4" s="3">
+        <v>0</v>
+      </c>
+      <c r="S4" s="3">
+        <v>0</v>
+      </c>
+      <c r="T4" s="3">
         <v>124</v>
       </c>
-      <c r="R4" s="3">
+      <c r="U4" s="3">
         <v>90</v>
       </c>
-      <c r="S4" s="3">
+      <c r="V4" s="3">
         <v>2.5</v>
       </c>
-      <c r="T4" s="3">
-        <v>0</v>
-      </c>
-      <c r="U4" s="7"/>
-    </row>
-    <row r="5" spans="1:21" ht="15" customHeight="1" thickBot="1">
+      <c r="W4" s="3">
+        <v>0</v>
+      </c>
+      <c r="X4" s="7"/>
+      <c r="Y4" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC4" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD4" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" ht="15" customHeight="1" thickBot="1">
       <c r="A5" s="12" t="s">
         <v>4</v>
       </c>
@@ -2910,23 +3025,50 @@
       <c r="P5" s="4">
         <v>0</v>
       </c>
-      <c r="Q5" s="4">
-        <v>0</v>
-      </c>
-      <c r="R5" s="4">
-        <v>0</v>
-      </c>
-      <c r="S5" s="4">
+      <c r="Q5" s="3">
+        <v>0</v>
+      </c>
+      <c r="R5" s="3">
+        <v>0</v>
+      </c>
+      <c r="S5" s="3">
         <v>0</v>
       </c>
       <c r="T5" s="4">
         <v>0</v>
       </c>
-      <c r="U5" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" ht="15" customHeight="1" thickBot="1">
+      <c r="U5" s="4">
+        <v>0</v>
+      </c>
+      <c r="V5" s="4">
+        <v>0</v>
+      </c>
+      <c r="W5" s="4">
+        <v>0</v>
+      </c>
+      <c r="X5" s="8">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC5" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD5" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" ht="15" customHeight="1" thickBot="1">
       <c r="A6" s="11" t="s">
         <v>5</v>
       </c>
@@ -2976,16 +3118,43 @@
         <v>4</v>
       </c>
       <c r="Q6" s="3">
+        <v>0</v>
+      </c>
+      <c r="R6" s="3">
+        <v>0</v>
+      </c>
+      <c r="S6" s="3">
+        <v>0</v>
+      </c>
+      <c r="T6" s="3">
         <v>70</v>
       </c>
-      <c r="R6" s="3">
+      <c r="U6" s="3">
         <v>34</v>
       </c>
-      <c r="S6" s="3"/>
-      <c r="T6" s="3"/>
-      <c r="U6" s="7"/>
-    </row>
-    <row r="7" spans="1:21" ht="15" customHeight="1" thickBot="1">
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+      <c r="X6" s="7"/>
+      <c r="Y6" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB6" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC6" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD6" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" ht="15" customHeight="1" thickBot="1">
       <c r="A7" s="11" t="s">
         <v>49</v>
       </c>
@@ -3035,20 +3204,47 @@
         <v>4</v>
       </c>
       <c r="Q7" s="3">
+        <v>0</v>
+      </c>
+      <c r="R7" s="3">
+        <v>0</v>
+      </c>
+      <c r="S7" s="3">
+        <v>0</v>
+      </c>
+      <c r="T7" s="3">
         <v>120</v>
       </c>
-      <c r="R7" s="3">
+      <c r="U7" s="3">
         <v>36</v>
       </c>
-      <c r="S7" s="3">
+      <c r="V7" s="3">
         <v>2.5</v>
       </c>
-      <c r="T7" s="3">
+      <c r="W7" s="3">
         <v>6</v>
       </c>
-      <c r="U7" s="7"/>
-    </row>
-    <row r="8" spans="1:21" ht="15" customHeight="1" thickBot="1">
+      <c r="X7" s="7"/>
+      <c r="Y7" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC7" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD7" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" ht="15" customHeight="1" thickBot="1">
       <c r="A8" s="15" t="s">
         <v>52</v>
       </c>
@@ -3097,21 +3293,48 @@
       <c r="P8" s="16">
         <v>4</v>
       </c>
-      <c r="Q8" s="16">
+      <c r="Q8" s="3">
+        <v>0</v>
+      </c>
+      <c r="R8" s="3">
+        <v>0</v>
+      </c>
+      <c r="S8" s="3">
+        <v>0</v>
+      </c>
+      <c r="T8" s="16">
         <v>90.5</v>
       </c>
-      <c r="R8" s="16">
+      <c r="U8" s="16">
         <v>58</v>
       </c>
-      <c r="S8" s="16">
+      <c r="V8" s="16">
         <v>2.5</v>
       </c>
-      <c r="T8" s="16">
-        <v>0</v>
-      </c>
-      <c r="U8" s="18"/>
-    </row>
-    <row r="9" spans="1:21" ht="15" customHeight="1" thickBot="1">
+      <c r="W8" s="16">
+        <v>0</v>
+      </c>
+      <c r="X8" s="18"/>
+      <c r="Y8" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD8" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30" ht="15" customHeight="1" thickBot="1">
       <c r="A9" s="10" t="s">
         <v>50</v>
       </c>
@@ -3161,20 +3384,47 @@
         <v>4</v>
       </c>
       <c r="Q9" s="3">
+        <v>0</v>
+      </c>
+      <c r="R9" s="3">
+        <v>0</v>
+      </c>
+      <c r="S9" s="3">
+        <v>0</v>
+      </c>
+      <c r="T9" s="3">
         <v>130.5</v>
       </c>
-      <c r="R9" s="1">
+      <c r="U9" s="1">
         <v>101</v>
       </c>
-      <c r="S9" s="3">
-        <v>0</v>
-      </c>
-      <c r="T9" s="1">
+      <c r="V9" s="3">
+        <v>0</v>
+      </c>
+      <c r="W9" s="1">
         <v>7</v>
       </c>
-      <c r="U9" s="7"/>
-    </row>
-    <row r="10" spans="1:21" ht="15" customHeight="1" thickBot="1">
+      <c r="X9" s="7"/>
+      <c r="Y9" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD9" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" ht="15" customHeight="1" thickBot="1">
       <c r="A10" s="10" t="s">
         <v>6</v>
       </c>
@@ -3224,20 +3474,47 @@
         <v>4</v>
       </c>
       <c r="Q10" s="3">
+        <v>0</v>
+      </c>
+      <c r="R10" s="3">
+        <v>0</v>
+      </c>
+      <c r="S10" s="3">
+        <v>0</v>
+      </c>
+      <c r="T10" s="3">
         <v>130</v>
       </c>
-      <c r="R10" s="3">
+      <c r="U10" s="3">
         <v>68</v>
       </c>
-      <c r="S10" s="3">
+      <c r="V10" s="3">
         <v>2.5</v>
       </c>
-      <c r="T10" s="3">
+      <c r="W10" s="3">
         <v>2</v>
       </c>
-      <c r="U10" s="7"/>
-    </row>
-    <row r="11" spans="1:21" ht="15" customHeight="1" thickBot="1">
+      <c r="X10" s="7"/>
+      <c r="Y10" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z10" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA10" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB10" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC10" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD10" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30" ht="15" customHeight="1" thickBot="1">
       <c r="A11" s="10" t="s">
         <v>7</v>
       </c>
@@ -3287,20 +3564,47 @@
         <v>4</v>
       </c>
       <c r="Q11" s="3">
+        <v>0</v>
+      </c>
+      <c r="R11" s="3">
+        <v>0</v>
+      </c>
+      <c r="S11" s="3">
+        <v>0</v>
+      </c>
+      <c r="T11" s="3">
         <v>107</v>
       </c>
-      <c r="R11" s="3">
+      <c r="U11" s="3">
         <v>78</v>
       </c>
-      <c r="S11" s="3">
+      <c r="V11" s="3">
         <v>2.5</v>
       </c>
-      <c r="T11" s="3">
+      <c r="W11" s="3">
         <v>2</v>
       </c>
-      <c r="U11" s="7"/>
-    </row>
-    <row r="12" spans="1:21" ht="15" customHeight="1" thickBot="1">
+      <c r="X11" s="7"/>
+      <c r="Y11" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z11" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA11" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB11" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC11" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD11" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30" ht="15" customHeight="1" thickBot="1">
       <c r="A12" s="12" t="s">
         <v>8</v>
       </c>
@@ -3349,23 +3653,50 @@
       <c r="P12" s="4">
         <v>0</v>
       </c>
-      <c r="Q12" s="4">
+      <c r="Q12" s="3">
+        <v>0</v>
+      </c>
+      <c r="R12" s="3">
+        <v>0</v>
+      </c>
+      <c r="S12" s="3">
+        <v>0</v>
+      </c>
+      <c r="T12" s="4">
         <v>2.5</v>
       </c>
-      <c r="R12" s="4">
+      <c r="U12" s="4">
         <v>3</v>
       </c>
-      <c r="S12" s="4">
-        <v>0</v>
-      </c>
-      <c r="T12" s="4">
-        <v>0</v>
-      </c>
-      <c r="U12" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" ht="15" customHeight="1" thickBot="1">
+      <c r="V12" s="4">
+        <v>0</v>
+      </c>
+      <c r="W12" s="4">
+        <v>0</v>
+      </c>
+      <c r="X12" s="8">
+        <v>0</v>
+      </c>
+      <c r="Y12" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z12" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA12" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB12" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC12" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD12" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" ht="15" customHeight="1" thickBot="1">
       <c r="A13" s="12" t="s">
         <v>9</v>
       </c>
@@ -3414,23 +3745,50 @@
       <c r="P13" s="4">
         <v>0</v>
       </c>
-      <c r="Q13" s="4">
-        <v>0</v>
-      </c>
-      <c r="R13" s="4">
-        <v>0</v>
-      </c>
-      <c r="S13" s="4">
+      <c r="Q13" s="3">
+        <v>0</v>
+      </c>
+      <c r="R13" s="3">
+        <v>0</v>
+      </c>
+      <c r="S13" s="3">
         <v>0</v>
       </c>
       <c r="T13" s="4">
         <v>0</v>
       </c>
-      <c r="U13" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" ht="15" customHeight="1" thickBot="1">
+      <c r="U13" s="4">
+        <v>0</v>
+      </c>
+      <c r="V13" s="4">
+        <v>0</v>
+      </c>
+      <c r="W13" s="4">
+        <v>0</v>
+      </c>
+      <c r="X13" s="8">
+        <v>0</v>
+      </c>
+      <c r="Y13" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z13" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA13" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB13" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC13" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD13" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" ht="15" customHeight="1" thickBot="1">
       <c r="A14" s="10" t="s">
         <v>10</v>
       </c>
@@ -3480,20 +3838,47 @@
         <v>4</v>
       </c>
       <c r="Q14" s="3">
+        <v>0</v>
+      </c>
+      <c r="R14" s="3">
+        <v>0</v>
+      </c>
+      <c r="S14" s="3">
+        <v>0</v>
+      </c>
+      <c r="T14" s="3">
         <v>152</v>
       </c>
-      <c r="R14" s="1">
+      <c r="U14" s="1">
         <v>28</v>
       </c>
-      <c r="S14" s="3">
+      <c r="V14" s="3">
         <v>3</v>
       </c>
-      <c r="T14" s="3">
-        <v>0</v>
-      </c>
-      <c r="U14" s="7"/>
-    </row>
-    <row r="15" spans="1:21" ht="15" customHeight="1" thickBot="1">
+      <c r="W14" s="3">
+        <v>0</v>
+      </c>
+      <c r="X14" s="7"/>
+      <c r="Y14" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z14" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA14" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB14" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC14" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD14" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30" ht="15" customHeight="1" thickBot="1">
       <c r="A15" s="10" t="s">
         <v>11</v>
       </c>
@@ -3543,20 +3928,47 @@
         <v>4</v>
       </c>
       <c r="Q15" s="3">
+        <v>0</v>
+      </c>
+      <c r="R15" s="3">
+        <v>0</v>
+      </c>
+      <c r="S15" s="3">
+        <v>0</v>
+      </c>
+      <c r="T15" s="3">
         <v>135</v>
       </c>
-      <c r="R15" s="3">
+      <c r="U15" s="3">
         <v>55</v>
       </c>
-      <c r="S15" s="3">
+      <c r="V15" s="3">
         <v>3</v>
       </c>
-      <c r="T15" s="3">
-        <v>0</v>
-      </c>
-      <c r="U15" s="7"/>
-    </row>
-    <row r="16" spans="1:21" ht="15" customHeight="1" thickBot="1">
+      <c r="W15" s="3">
+        <v>0</v>
+      </c>
+      <c r="X15" s="7"/>
+      <c r="Y15" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z15" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA15" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB15" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC15" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD15" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30" ht="15" customHeight="1" thickBot="1">
       <c r="A16" s="12" t="s">
         <v>12</v>
       </c>
@@ -3605,23 +4017,50 @@
       <c r="P16" s="4">
         <v>0</v>
       </c>
-      <c r="Q16" s="4">
-        <v>0</v>
-      </c>
-      <c r="R16" s="4">
-        <v>0</v>
-      </c>
-      <c r="S16" s="4">
+      <c r="Q16" s="3">
+        <v>0</v>
+      </c>
+      <c r="R16" s="3">
+        <v>0</v>
+      </c>
+      <c r="S16" s="3">
         <v>0</v>
       </c>
       <c r="T16" s="4">
         <v>0</v>
       </c>
-      <c r="U16" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:21" ht="15" customHeight="1" thickBot="1">
+      <c r="U16" s="4">
+        <v>0</v>
+      </c>
+      <c r="V16" s="4">
+        <v>0</v>
+      </c>
+      <c r="W16" s="4">
+        <v>0</v>
+      </c>
+      <c r="X16" s="8">
+        <v>0</v>
+      </c>
+      <c r="Y16" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z16" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA16" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB16" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC16" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD16" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:30" ht="15" customHeight="1" thickBot="1">
       <c r="A17" s="10" t="s">
         <v>13</v>
       </c>
@@ -3671,20 +4110,47 @@
         <v>4</v>
       </c>
       <c r="Q17" s="3">
+        <v>0</v>
+      </c>
+      <c r="R17" s="3">
+        <v>0</v>
+      </c>
+      <c r="S17" s="3">
+        <v>0</v>
+      </c>
+      <c r="T17" s="3">
         <v>101</v>
       </c>
-      <c r="R17" s="3">
+      <c r="U17" s="3">
         <v>99</v>
       </c>
-      <c r="S17" s="3">
+      <c r="V17" s="3">
         <v>2.5</v>
       </c>
-      <c r="T17" s="3">
+      <c r="W17" s="3">
         <v>1</v>
       </c>
-      <c r="U17" s="7"/>
-    </row>
-    <row r="18" spans="1:21" ht="15" customHeight="1" thickBot="1">
+      <c r="X17" s="7"/>
+      <c r="Y17" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z17" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA17" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB17" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC17" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD17" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:30" ht="15" customHeight="1" thickBot="1">
       <c r="A18" s="12" t="s">
         <v>14</v>
       </c>
@@ -3733,23 +4199,50 @@
       <c r="P18" s="4">
         <v>0</v>
       </c>
-      <c r="Q18" s="4">
-        <v>0</v>
-      </c>
-      <c r="R18" s="4">
-        <v>0</v>
-      </c>
-      <c r="S18" s="4">
+      <c r="Q18" s="3">
+        <v>0</v>
+      </c>
+      <c r="R18" s="3">
+        <v>0</v>
+      </c>
+      <c r="S18" s="3">
         <v>0</v>
       </c>
       <c r="T18" s="4">
         <v>0</v>
       </c>
-      <c r="U18" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21" ht="15" customHeight="1" thickBot="1">
+      <c r="U18" s="4">
+        <v>0</v>
+      </c>
+      <c r="V18" s="4">
+        <v>0</v>
+      </c>
+      <c r="W18" s="4">
+        <v>0</v>
+      </c>
+      <c r="X18" s="8">
+        <v>0</v>
+      </c>
+      <c r="Y18" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z18" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA18" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB18" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC18" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD18" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:30" ht="15" customHeight="1" thickBot="1">
       <c r="A19" s="10" t="s">
         <v>15</v>
       </c>
@@ -3798,21 +4291,48 @@
       <c r="P19" s="3">
         <v>4</v>
       </c>
-      <c r="Q19" s="1">
+      <c r="Q19" s="3">
+        <v>0</v>
+      </c>
+      <c r="R19" s="3">
+        <v>0</v>
+      </c>
+      <c r="S19" s="3">
+        <v>0</v>
+      </c>
+      <c r="T19" s="1">
         <v>130</v>
       </c>
-      <c r="R19" s="1">
+      <c r="U19" s="1">
         <v>78</v>
       </c>
-      <c r="S19" s="3">
-        <v>0</v>
-      </c>
-      <c r="T19" s="3">
-        <v>0</v>
-      </c>
-      <c r="U19" s="7"/>
-    </row>
-    <row r="20" spans="1:21" ht="15" customHeight="1" thickBot="1">
+      <c r="V19" s="3">
+        <v>0</v>
+      </c>
+      <c r="W19" s="3">
+        <v>0</v>
+      </c>
+      <c r="X19" s="7"/>
+      <c r="Y19" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z19" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA19" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB19" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC19" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD19" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:30" ht="15" customHeight="1" thickBot="1">
       <c r="A20" s="12" t="s">
         <v>16</v>
       </c>
@@ -3861,23 +4381,50 @@
       <c r="P20" s="4">
         <v>0</v>
       </c>
-      <c r="Q20" s="4">
-        <v>0</v>
-      </c>
-      <c r="R20" s="4">
-        <v>0</v>
-      </c>
-      <c r="S20" s="4">
+      <c r="Q20" s="3">
+        <v>0</v>
+      </c>
+      <c r="R20" s="3">
+        <v>0</v>
+      </c>
+      <c r="S20" s="3">
         <v>0</v>
       </c>
       <c r="T20" s="4">
         <v>0</v>
       </c>
-      <c r="U20" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21" ht="15" customHeight="1" thickBot="1">
+      <c r="U20" s="4">
+        <v>0</v>
+      </c>
+      <c r="V20" s="4">
+        <v>0</v>
+      </c>
+      <c r="W20" s="4">
+        <v>0</v>
+      </c>
+      <c r="X20" s="8">
+        <v>0</v>
+      </c>
+      <c r="Y20" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z20" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA20" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB20" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC20" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD20" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:30" ht="15" customHeight="1" thickBot="1">
       <c r="A21" s="10" t="s">
         <v>17</v>
       </c>
@@ -3927,20 +4474,47 @@
         <v>4</v>
       </c>
       <c r="Q21" s="3">
+        <v>0</v>
+      </c>
+      <c r="R21" s="3">
+        <v>0</v>
+      </c>
+      <c r="S21" s="3">
+        <v>0</v>
+      </c>
+      <c r="T21" s="3">
         <v>95</v>
       </c>
-      <c r="R21" s="3">
+      <c r="U21" s="3">
         <v>78</v>
       </c>
-      <c r="S21" s="3">
+      <c r="V21" s="3">
         <v>2.5</v>
       </c>
-      <c r="T21" s="3">
-        <v>0</v>
-      </c>
-      <c r="U21" s="7"/>
-    </row>
-    <row r="22" spans="1:21" ht="15" customHeight="1" thickBot="1">
+      <c r="W21" s="3">
+        <v>0</v>
+      </c>
+      <c r="X21" s="7"/>
+      <c r="Y21" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z21" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA21" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB21" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC21" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD21" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:30" ht="15" customHeight="1" thickBot="1">
       <c r="A22" s="10" t="s">
         <v>18</v>
       </c>
@@ -3990,20 +4564,47 @@
         <v>4</v>
       </c>
       <c r="Q22" s="3">
+        <v>0</v>
+      </c>
+      <c r="R22" s="3">
+        <v>0</v>
+      </c>
+      <c r="S22" s="3">
+        <v>0</v>
+      </c>
+      <c r="T22" s="3">
         <v>116</v>
       </c>
-      <c r="R22" s="3">
+      <c r="U22" s="3">
         <v>92</v>
       </c>
-      <c r="S22" s="3">
+      <c r="V22" s="3">
         <v>2.5</v>
       </c>
-      <c r="T22" s="3">
+      <c r="W22" s="3">
         <v>2</v>
       </c>
-      <c r="U22" s="7"/>
-    </row>
-    <row r="23" spans="1:21" ht="15" customHeight="1" thickBot="1">
+      <c r="X22" s="7"/>
+      <c r="Y22" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z22" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA22" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB22" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC22" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD22" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:30" ht="15" customHeight="1" thickBot="1">
       <c r="A23" s="10" t="s">
         <v>53</v>
       </c>
@@ -4052,21 +4653,48 @@
       <c r="P23" s="22">
         <v>4</v>
       </c>
-      <c r="Q23" s="22">
+      <c r="Q23" s="3">
+        <v>0</v>
+      </c>
+      <c r="R23" s="3">
+        <v>0</v>
+      </c>
+      <c r="S23" s="3">
+        <v>0</v>
+      </c>
+      <c r="T23" s="22">
         <v>130</v>
       </c>
-      <c r="R23" s="22">
+      <c r="U23" s="22">
         <v>82</v>
       </c>
-      <c r="S23" s="22">
+      <c r="V23" s="22">
         <v>3</v>
       </c>
-      <c r="T23" s="22">
+      <c r="W23" s="22">
         <v>2</v>
       </c>
-      <c r="U23" s="24"/>
-    </row>
-    <row r="24" spans="1:21" ht="15" customHeight="1" thickBot="1">
+      <c r="X23" s="24"/>
+      <c r="Y23" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z23" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA23" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB23" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC23" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD23" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:30" ht="15" customHeight="1" thickBot="1">
       <c r="A24" s="10" t="s">
         <v>19</v>
       </c>
@@ -4116,22 +4744,49 @@
         <v>4</v>
       </c>
       <c r="Q24" s="3">
+        <v>0</v>
+      </c>
+      <c r="R24" s="3">
+        <v>0</v>
+      </c>
+      <c r="S24" s="3">
+        <v>0</v>
+      </c>
+      <c r="T24" s="3">
         <v>100</v>
       </c>
-      <c r="R24" s="3">
+      <c r="U24" s="3">
         <v>70</v>
       </c>
-      <c r="S24" s="3">
+      <c r="V24" s="3">
         <v>2.5</v>
       </c>
-      <c r="T24" s="3">
-        <v>0</v>
-      </c>
-      <c r="U24" s="7">
+      <c r="W24" s="3">
+        <v>0</v>
+      </c>
+      <c r="X24" s="7">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:21" ht="15" customHeight="1" thickBot="1">
+      <c r="Y24" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z24" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA24" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB24" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC24" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD24" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:30" ht="15" customHeight="1" thickBot="1">
       <c r="A25" s="10" t="s">
         <v>20</v>
       </c>
@@ -4181,20 +4836,47 @@
         <v>4</v>
       </c>
       <c r="Q25" s="3">
+        <v>0</v>
+      </c>
+      <c r="R25" s="3">
+        <v>0</v>
+      </c>
+      <c r="S25" s="3">
+        <v>0</v>
+      </c>
+      <c r="T25" s="3">
         <v>129.5</v>
       </c>
-      <c r="R25" s="3">
+      <c r="U25" s="3">
         <v>90</v>
       </c>
-      <c r="S25" s="3">
+      <c r="V25" s="3">
         <v>3</v>
       </c>
-      <c r="T25" s="3">
-        <v>0</v>
-      </c>
-      <c r="U25" s="7"/>
-    </row>
-    <row r="26" spans="1:21" ht="15" customHeight="1" thickBot="1">
+      <c r="W25" s="3">
+        <v>0</v>
+      </c>
+      <c r="X25" s="7"/>
+      <c r="Y25" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z25" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA25" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB25" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC25" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD25" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:30" ht="15" customHeight="1" thickBot="1">
       <c r="A26" s="10" t="s">
         <v>51</v>
       </c>
@@ -4244,20 +4926,47 @@
         <v>4</v>
       </c>
       <c r="Q26" s="3">
+        <v>0</v>
+      </c>
+      <c r="R26" s="3">
+        <v>0</v>
+      </c>
+      <c r="S26" s="3">
+        <v>0</v>
+      </c>
+      <c r="T26" s="3">
         <v>17</v>
       </c>
-      <c r="R26" s="3">
+      <c r="U26" s="3">
         <v>2</v>
       </c>
-      <c r="S26" s="3">
+      <c r="V26" s="3">
         <v>2</v>
       </c>
-      <c r="T26" s="3">
-        <v>0</v>
-      </c>
-      <c r="U26" s="7"/>
-    </row>
-    <row r="27" spans="1:21" ht="15" customHeight="1" thickBot="1">
+      <c r="W26" s="3">
+        <v>0</v>
+      </c>
+      <c r="X26" s="7"/>
+      <c r="Y26" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z26" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA26" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB26" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC26" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD26" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:30" ht="15" customHeight="1" thickBot="1">
       <c r="A27" s="10" t="s">
         <v>21</v>
       </c>
@@ -4307,20 +5016,47 @@
         <v>4</v>
       </c>
       <c r="Q27" s="3">
+        <v>0</v>
+      </c>
+      <c r="R27" s="3">
+        <v>0</v>
+      </c>
+      <c r="S27" s="3">
+        <v>0</v>
+      </c>
+      <c r="T27" s="3">
         <v>101</v>
       </c>
-      <c r="R27" s="1">
+      <c r="U27" s="1">
         <v>83</v>
       </c>
-      <c r="S27" s="3">
+      <c r="V27" s="3">
         <v>0.5</v>
       </c>
-      <c r="T27" s="3">
+      <c r="W27" s="3">
         <v>1</v>
       </c>
-      <c r="U27" s="7"/>
-    </row>
-    <row r="28" spans="1:21" ht="15" customHeight="1" thickBot="1">
+      <c r="X27" s="7"/>
+      <c r="Y27" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z27" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA27" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB27" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC27" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD27" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:30" ht="15" customHeight="1" thickBot="1">
       <c r="A28" s="10" t="s">
         <v>22</v>
       </c>
@@ -4370,20 +5106,47 @@
         <v>4</v>
       </c>
       <c r="Q28" s="3">
+        <v>0</v>
+      </c>
+      <c r="R28" s="3">
+        <v>0</v>
+      </c>
+      <c r="S28" s="3">
+        <v>0</v>
+      </c>
+      <c r="T28" s="3">
         <v>128</v>
       </c>
-      <c r="R28" s="3">
+      <c r="U28" s="3">
         <v>70</v>
       </c>
-      <c r="S28" s="3">
+      <c r="V28" s="3">
         <v>2.5</v>
       </c>
-      <c r="T28" s="3">
+      <c r="W28" s="3">
         <v>1</v>
       </c>
-      <c r="U28" s="7"/>
-    </row>
-    <row r="29" spans="1:21" ht="15" customHeight="1" thickBot="1">
+      <c r="X28" s="7"/>
+      <c r="Y28" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z28" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA28" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB28" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC28" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD28" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:30" ht="15" customHeight="1" thickBot="1">
       <c r="A29" s="10" t="s">
         <v>23</v>
       </c>
@@ -4433,20 +5196,47 @@
         <v>4</v>
       </c>
       <c r="Q29" s="3">
+        <v>0</v>
+      </c>
+      <c r="R29" s="3">
+        <v>0</v>
+      </c>
+      <c r="S29" s="3">
+        <v>0</v>
+      </c>
+      <c r="T29" s="3">
         <v>112</v>
       </c>
-      <c r="R29" s="3">
+      <c r="U29" s="3">
         <v>90</v>
       </c>
-      <c r="S29" s="3">
+      <c r="V29" s="3">
         <v>2.5</v>
       </c>
-      <c r="T29" s="3">
+      <c r="W29" s="3">
         <v>1</v>
       </c>
-      <c r="U29" s="7"/>
-    </row>
-    <row r="30" spans="1:21" ht="15" customHeight="1" thickBot="1">
+      <c r="X29" s="7"/>
+      <c r="Y29" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z29" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA29" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB29" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC29" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD29" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:30" ht="15" customHeight="1" thickBot="1">
       <c r="A30" s="12" t="s">
         <v>24</v>
       </c>
@@ -4495,23 +5285,50 @@
       <c r="P30" s="4">
         <v>0</v>
       </c>
-      <c r="Q30" s="4">
-        <v>0</v>
-      </c>
-      <c r="R30" s="4">
-        <v>0</v>
-      </c>
-      <c r="S30" s="4">
+      <c r="Q30" s="3">
+        <v>0</v>
+      </c>
+      <c r="R30" s="3">
+        <v>0</v>
+      </c>
+      <c r="S30" s="3">
         <v>0</v>
       </c>
       <c r="T30" s="4">
         <v>0</v>
       </c>
-      <c r="U30" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:21" ht="15" customHeight="1" thickBot="1">
+      <c r="U30" s="4">
+        <v>0</v>
+      </c>
+      <c r="V30" s="4">
+        <v>0</v>
+      </c>
+      <c r="W30" s="4">
+        <v>0</v>
+      </c>
+      <c r="X30" s="8">
+        <v>0</v>
+      </c>
+      <c r="Y30" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z30" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA30" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB30" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC30" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD30" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:30" ht="15" customHeight="1" thickBot="1">
       <c r="A31" s="10" t="s">
         <v>25</v>
       </c>
@@ -4561,20 +5378,47 @@
         <v>4</v>
       </c>
       <c r="Q31" s="3">
+        <v>0</v>
+      </c>
+      <c r="R31" s="3">
+        <v>0</v>
+      </c>
+      <c r="S31" s="3">
+        <v>0</v>
+      </c>
+      <c r="T31" s="3">
         <v>109</v>
       </c>
-      <c r="R31" s="3">
+      <c r="U31" s="3">
         <v>70</v>
       </c>
-      <c r="S31" s="3">
+      <c r="V31" s="3">
         <v>2.5</v>
       </c>
-      <c r="T31" s="3">
-        <v>0</v>
-      </c>
-      <c r="U31" s="7"/>
-    </row>
-    <row r="32" spans="1:21" ht="15" customHeight="1" thickBot="1">
+      <c r="W31" s="3">
+        <v>0</v>
+      </c>
+      <c r="X31" s="7"/>
+      <c r="Y31" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z31" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA31" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB31" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC31" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD31" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:30" ht="15" customHeight="1" thickBot="1">
       <c r="A32" s="12" t="s">
         <v>26</v>
       </c>
@@ -4623,23 +5467,50 @@
       <c r="P32" s="4">
         <v>0</v>
       </c>
-      <c r="Q32" s="4">
-        <v>0</v>
-      </c>
-      <c r="R32" s="4">
-        <v>0</v>
-      </c>
-      <c r="S32" s="4">
+      <c r="Q32" s="3">
+        <v>0</v>
+      </c>
+      <c r="R32" s="3">
+        <v>0</v>
+      </c>
+      <c r="S32" s="3">
         <v>0</v>
       </c>
       <c r="T32" s="4">
         <v>0</v>
       </c>
-      <c r="U32" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:21" ht="15" customHeight="1" thickBot="1">
+      <c r="U32" s="4">
+        <v>0</v>
+      </c>
+      <c r="V32" s="4">
+        <v>0</v>
+      </c>
+      <c r="W32" s="4">
+        <v>0</v>
+      </c>
+      <c r="X32" s="8">
+        <v>0</v>
+      </c>
+      <c r="Y32" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z32" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA32" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB32" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC32" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD32" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:30" ht="15" customHeight="1" thickBot="1">
       <c r="A33" s="12" t="s">
         <v>27</v>
       </c>
@@ -4688,23 +5559,50 @@
       <c r="P33" s="4">
         <v>0</v>
       </c>
-      <c r="Q33" s="4">
-        <v>0</v>
-      </c>
-      <c r="R33" s="4">
-        <v>0</v>
-      </c>
-      <c r="S33" s="4">
+      <c r="Q33" s="3">
+        <v>0</v>
+      </c>
+      <c r="R33" s="3">
+        <v>0</v>
+      </c>
+      <c r="S33" s="3">
         <v>0</v>
       </c>
       <c r="T33" s="4">
         <v>0</v>
       </c>
-      <c r="U33" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:21" ht="15" customHeight="1" thickBot="1">
+      <c r="U33" s="4">
+        <v>0</v>
+      </c>
+      <c r="V33" s="4">
+        <v>0</v>
+      </c>
+      <c r="W33" s="4">
+        <v>0</v>
+      </c>
+      <c r="X33" s="8">
+        <v>0</v>
+      </c>
+      <c r="Y33" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z33" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA33" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB33" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC33" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD33" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:30" ht="15" customHeight="1" thickBot="1">
       <c r="A34" s="10" t="s">
         <v>28</v>
       </c>
@@ -4754,20 +5652,47 @@
         <v>4</v>
       </c>
       <c r="Q34" s="3">
+        <v>0</v>
+      </c>
+      <c r="R34" s="3">
+        <v>0</v>
+      </c>
+      <c r="S34" s="3">
+        <v>0</v>
+      </c>
+      <c r="T34" s="3">
         <v>106.5</v>
       </c>
-      <c r="R34" s="3">
+      <c r="U34" s="3">
         <v>87</v>
       </c>
-      <c r="S34" s="3">
+      <c r="V34" s="3">
         <v>2.5</v>
       </c>
-      <c r="T34" s="3">
-        <v>0</v>
-      </c>
-      <c r="U34" s="7"/>
-    </row>
-    <row r="35" spans="1:21" ht="15" customHeight="1" thickBot="1">
+      <c r="W34" s="3">
+        <v>0</v>
+      </c>
+      <c r="X34" s="7"/>
+      <c r="Y34" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z34" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA34" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB34" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC34" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD34" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:30" ht="15" customHeight="1" thickBot="1">
       <c r="A35" s="10" t="s">
         <v>29</v>
       </c>
@@ -4816,21 +5741,48 @@
       <c r="P35" s="3">
         <v>4</v>
       </c>
-      <c r="Q35" s="1">
+      <c r="Q35" s="3">
+        <v>0</v>
+      </c>
+      <c r="R35" s="3">
+        <v>0</v>
+      </c>
+      <c r="S35" s="3">
+        <v>0</v>
+      </c>
+      <c r="T35" s="1">
         <v>128</v>
       </c>
-      <c r="R35" s="1">
+      <c r="U35" s="1">
         <v>138</v>
       </c>
-      <c r="S35" s="3">
-        <v>0</v>
-      </c>
-      <c r="T35" s="3">
+      <c r="V35" s="3">
+        <v>0</v>
+      </c>
+      <c r="W35" s="3">
         <v>6</v>
       </c>
-      <c r="U35" s="7"/>
-    </row>
-    <row r="36" spans="1:21" ht="15" customHeight="1" thickBot="1">
+      <c r="X35" s="7"/>
+      <c r="Y35" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z35" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA35" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB35" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC35" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD35" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:30" ht="15" customHeight="1" thickBot="1">
       <c r="A36" s="10" t="s">
         <v>30</v>
       </c>
@@ -4880,20 +5832,47 @@
         <v>4</v>
       </c>
       <c r="Q36" s="3">
+        <v>0</v>
+      </c>
+      <c r="R36" s="3">
+        <v>0</v>
+      </c>
+      <c r="S36" s="3">
+        <v>0</v>
+      </c>
+      <c r="T36" s="3">
         <v>114</v>
       </c>
-      <c r="R36" s="3">
+      <c r="U36" s="3">
         <v>90</v>
       </c>
-      <c r="S36" s="3">
+      <c r="V36" s="3">
         <v>2.5</v>
       </c>
-      <c r="T36" s="3">
-        <v>0</v>
-      </c>
-      <c r="U36" s="7"/>
-    </row>
-    <row r="37" spans="1:21" ht="15" customHeight="1" thickBot="1">
+      <c r="W36" s="3">
+        <v>0</v>
+      </c>
+      <c r="X36" s="7"/>
+      <c r="Y36" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z36" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA36" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB36" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC36" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD36" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:30" ht="15" customHeight="1" thickBot="1">
       <c r="A37" s="10" t="s">
         <v>31</v>
       </c>
@@ -4943,20 +5922,47 @@
         <v>4</v>
       </c>
       <c r="Q37" s="3">
+        <v>0</v>
+      </c>
+      <c r="R37" s="3">
+        <v>0</v>
+      </c>
+      <c r="S37" s="3">
+        <v>0</v>
+      </c>
+      <c r="T37" s="3">
         <v>4</v>
       </c>
-      <c r="R37" s="3">
+      <c r="U37" s="3">
         <v>10</v>
       </c>
-      <c r="S37" s="3">
-        <v>0</v>
-      </c>
-      <c r="T37" s="3">
-        <v>0</v>
-      </c>
-      <c r="U37" s="7"/>
-    </row>
-    <row r="38" spans="1:21" ht="15" customHeight="1" thickBot="1">
+      <c r="V37" s="3">
+        <v>0</v>
+      </c>
+      <c r="W37" s="3">
+        <v>0</v>
+      </c>
+      <c r="X37" s="7"/>
+      <c r="Y37" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z37" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA37" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB37" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC37" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD37" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:30" ht="15" customHeight="1" thickBot="1">
       <c r="A38" s="10" t="s">
         <v>32</v>
       </c>
@@ -5005,21 +6011,48 @@
       <c r="P38" s="3">
         <v>4</v>
       </c>
-      <c r="Q38" s="1">
+      <c r="Q38" s="3">
+        <v>0</v>
+      </c>
+      <c r="R38" s="3">
+        <v>0</v>
+      </c>
+      <c r="S38" s="3">
+        <v>0</v>
+      </c>
+      <c r="T38" s="1">
         <v>141.5</v>
       </c>
-      <c r="R38" s="1">
+      <c r="U38" s="1">
         <v>94</v>
       </c>
-      <c r="S38" s="3">
+      <c r="V38" s="3">
         <v>2.5</v>
       </c>
-      <c r="T38" s="3">
-        <v>0</v>
-      </c>
-      <c r="U38" s="7"/>
-    </row>
-    <row r="39" spans="1:21" ht="15" customHeight="1" thickBot="1">
+      <c r="W38" s="3">
+        <v>0</v>
+      </c>
+      <c r="X38" s="7"/>
+      <c r="Y38" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z38" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA38" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB38" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC38" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD38" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:30" ht="15" customHeight="1" thickBot="1">
       <c r="A39" s="10" t="s">
         <v>33</v>
       </c>
@@ -5069,20 +6102,47 @@
         <v>4</v>
       </c>
       <c r="Q39" s="3">
+        <v>0</v>
+      </c>
+      <c r="R39" s="3">
+        <v>0</v>
+      </c>
+      <c r="S39" s="3">
+        <v>0</v>
+      </c>
+      <c r="T39" s="3">
         <v>95</v>
       </c>
-      <c r="R39" s="3">
+      <c r="U39" s="3">
         <v>86</v>
       </c>
-      <c r="S39" s="1">
+      <c r="V39" s="1">
         <v>2.5</v>
       </c>
-      <c r="T39" s="3">
+      <c r="W39" s="3">
         <v>6</v>
       </c>
-      <c r="U39" s="7"/>
-    </row>
-    <row r="40" spans="1:21" ht="15" customHeight="1" thickBot="1">
+      <c r="X39" s="7"/>
+      <c r="Y39" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z39" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA39" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB39" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC39" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD39" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:30" ht="15" customHeight="1" thickBot="1">
       <c r="A40" s="10" t="s">
         <v>34</v>
       </c>
@@ -5132,20 +6192,47 @@
         <v>4</v>
       </c>
       <c r="Q40" s="3">
+        <v>0</v>
+      </c>
+      <c r="R40" s="3">
+        <v>0</v>
+      </c>
+      <c r="S40" s="3">
+        <v>0</v>
+      </c>
+      <c r="T40" s="3">
         <v>103</v>
       </c>
-      <c r="R40" s="3">
+      <c r="U40" s="3">
         <v>83</v>
       </c>
-      <c r="S40" s="3">
-        <v>0</v>
-      </c>
-      <c r="T40" s="3">
-        <v>0</v>
-      </c>
-      <c r="U40" s="7"/>
-    </row>
-    <row r="41" spans="1:21" ht="15" customHeight="1" thickBot="1">
+      <c r="V40" s="3">
+        <v>0</v>
+      </c>
+      <c r="W40" s="3">
+        <v>0</v>
+      </c>
+      <c r="X40" s="7"/>
+      <c r="Y40" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z40" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA40" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB40" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC40" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD40" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:30" ht="15" customHeight="1" thickBot="1">
       <c r="A41" s="12" t="s">
         <v>35</v>
       </c>
@@ -5194,23 +6281,50 @@
       <c r="P41" s="4">
         <v>0</v>
       </c>
-      <c r="Q41" s="4">
-        <v>0</v>
-      </c>
-      <c r="R41" s="4">
-        <v>0</v>
-      </c>
-      <c r="S41" s="4">
+      <c r="Q41" s="3">
+        <v>0</v>
+      </c>
+      <c r="R41" s="3">
+        <v>0</v>
+      </c>
+      <c r="S41" s="3">
         <v>0</v>
       </c>
       <c r="T41" s="4">
         <v>0</v>
       </c>
-      <c r="U41" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:21" ht="15" customHeight="1" thickBot="1">
+      <c r="U41" s="4">
+        <v>0</v>
+      </c>
+      <c r="V41" s="4">
+        <v>0</v>
+      </c>
+      <c r="W41" s="4">
+        <v>0</v>
+      </c>
+      <c r="X41" s="8">
+        <v>0</v>
+      </c>
+      <c r="Y41" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z41" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA41" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB41" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC41" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD41" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:30" ht="15" customHeight="1" thickBot="1">
       <c r="A42" s="10" t="s">
         <v>36</v>
       </c>
@@ -5260,20 +6374,47 @@
         <v>4</v>
       </c>
       <c r="Q42" s="3">
+        <v>0</v>
+      </c>
+      <c r="R42" s="3">
+        <v>0</v>
+      </c>
+      <c r="S42" s="3">
+        <v>0</v>
+      </c>
+      <c r="T42" s="3">
         <v>18</v>
       </c>
-      <c r="R42" s="3">
+      <c r="U42" s="3">
         <v>15</v>
       </c>
-      <c r="S42" s="3">
-        <v>0</v>
-      </c>
-      <c r="T42" s="3">
-        <v>0</v>
-      </c>
-      <c r="U42" s="7"/>
-    </row>
-    <row r="43" spans="1:21" ht="15" customHeight="1" thickBot="1">
+      <c r="V42" s="3">
+        <v>0</v>
+      </c>
+      <c r="W42" s="3">
+        <v>0</v>
+      </c>
+      <c r="X42" s="7"/>
+      <c r="Y42" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z42" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA42" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB42" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC42" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD42" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:30" ht="15" customHeight="1" thickBot="1">
       <c r="A43" s="12" t="s">
         <v>37</v>
       </c>
@@ -5322,23 +6463,50 @@
       <c r="P43" s="4">
         <v>0</v>
       </c>
-      <c r="Q43" s="4">
-        <v>0</v>
-      </c>
-      <c r="R43" s="4">
-        <v>0</v>
-      </c>
-      <c r="S43" s="4">
+      <c r="Q43" s="3">
+        <v>0</v>
+      </c>
+      <c r="R43" s="3">
+        <v>0</v>
+      </c>
+      <c r="S43" s="3">
         <v>0</v>
       </c>
       <c r="T43" s="4">
         <v>0</v>
       </c>
-      <c r="U43" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:21" ht="15" customHeight="1" thickBot="1">
+      <c r="U43" s="4">
+        <v>0</v>
+      </c>
+      <c r="V43" s="4">
+        <v>0</v>
+      </c>
+      <c r="W43" s="4">
+        <v>0</v>
+      </c>
+      <c r="X43" s="8">
+        <v>0</v>
+      </c>
+      <c r="Y43" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z43" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA43" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB43" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC43" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD43" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:30" ht="15" customHeight="1" thickBot="1">
       <c r="A44" s="12" t="s">
         <v>38</v>
       </c>
@@ -5387,23 +6555,50 @@
       <c r="P44" s="4">
         <v>0</v>
       </c>
-      <c r="Q44" s="4">
-        <v>0</v>
-      </c>
-      <c r="R44" s="4">
-        <v>0</v>
-      </c>
-      <c r="S44" s="4">
+      <c r="Q44" s="3">
+        <v>0</v>
+      </c>
+      <c r="R44" s="3">
+        <v>0</v>
+      </c>
+      <c r="S44" s="3">
         <v>0</v>
       </c>
       <c r="T44" s="4">
         <v>0</v>
       </c>
-      <c r="U44" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:21" ht="15" customHeight="1" thickBot="1">
+      <c r="U44" s="4">
+        <v>0</v>
+      </c>
+      <c r="V44" s="4">
+        <v>0</v>
+      </c>
+      <c r="W44" s="4">
+        <v>0</v>
+      </c>
+      <c r="X44" s="8">
+        <v>0</v>
+      </c>
+      <c r="Y44" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z44" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA44" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB44" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC44" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD44" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:30" ht="15" customHeight="1" thickBot="1">
       <c r="A45" s="10" t="s">
         <v>39</v>
       </c>
@@ -5452,21 +6647,48 @@
       <c r="P45" s="3">
         <v>5</v>
       </c>
-      <c r="Q45" s="6">
+      <c r="Q45" s="3">
+        <v>0</v>
+      </c>
+      <c r="R45" s="3">
+        <v>0</v>
+      </c>
+      <c r="S45" s="3">
+        <v>0</v>
+      </c>
+      <c r="T45" s="6">
         <v>208</v>
       </c>
-      <c r="R45" s="1">
+      <c r="U45" s="1">
         <v>112</v>
       </c>
-      <c r="S45" s="3">
-        <v>0</v>
-      </c>
-      <c r="T45" s="3">
-        <v>0</v>
-      </c>
-      <c r="U45" s="7"/>
-    </row>
-    <row r="46" spans="1:21" ht="15" customHeight="1" thickBot="1">
+      <c r="V45" s="3">
+        <v>0</v>
+      </c>
+      <c r="W45" s="3">
+        <v>0</v>
+      </c>
+      <c r="X45" s="7"/>
+      <c r="Y45" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z45" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA45" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB45" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC45" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD45" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:30" ht="15" customHeight="1" thickBot="1">
       <c r="A46" s="10" t="s">
         <v>40</v>
       </c>
@@ -5515,21 +6737,48 @@
       <c r="P46" s="3">
         <v>4</v>
       </c>
-      <c r="Q46" s="1">
+      <c r="Q46" s="3">
+        <v>0</v>
+      </c>
+      <c r="R46" s="3">
+        <v>0</v>
+      </c>
+      <c r="S46" s="3">
+        <v>0</v>
+      </c>
+      <c r="T46" s="1">
         <v>148.5</v>
       </c>
-      <c r="R46" s="1">
+      <c r="U46" s="1">
         <v>119</v>
       </c>
-      <c r="S46" s="3">
-        <v>0</v>
-      </c>
-      <c r="T46" s="3">
-        <v>0</v>
-      </c>
-      <c r="U46" s="7"/>
-    </row>
-    <row r="47" spans="1:21" ht="15" customHeight="1" thickBot="1">
+      <c r="V46" s="3">
+        <v>0</v>
+      </c>
+      <c r="W46" s="3">
+        <v>0</v>
+      </c>
+      <c r="X46" s="7"/>
+      <c r="Y46" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z46" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA46" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB46" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC46" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD46" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:30" ht="15" customHeight="1" thickBot="1">
       <c r="A47" s="10" t="s">
         <v>41</v>
       </c>
@@ -5578,21 +6827,48 @@
       <c r="P47" s="3">
         <v>4</v>
       </c>
-      <c r="Q47" s="1">
+      <c r="Q47" s="3">
+        <v>0</v>
+      </c>
+      <c r="R47" s="3">
+        <v>0</v>
+      </c>
+      <c r="S47" s="3">
+        <v>0</v>
+      </c>
+      <c r="T47" s="1">
         <v>130</v>
       </c>
-      <c r="R47" s="1">
+      <c r="U47" s="1">
         <v>96</v>
       </c>
-      <c r="S47" s="3">
-        <v>0</v>
-      </c>
-      <c r="T47" s="3">
-        <v>0</v>
-      </c>
-      <c r="U47" s="7"/>
-    </row>
-    <row r="48" spans="1:21" ht="15" customHeight="1" thickBot="1">
+      <c r="V47" s="3">
+        <v>0</v>
+      </c>
+      <c r="W47" s="3">
+        <v>0</v>
+      </c>
+      <c r="X47" s="7"/>
+      <c r="Y47" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z47" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA47" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB47" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC47" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD47" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:30" ht="15" customHeight="1" thickBot="1">
       <c r="A48" s="10" t="s">
         <v>42</v>
       </c>
@@ -5641,21 +6917,48 @@
       <c r="P48" s="3">
         <v>4</v>
       </c>
-      <c r="Q48" s="1">
+      <c r="Q48" s="3">
+        <v>0</v>
+      </c>
+      <c r="R48" s="3">
+        <v>0</v>
+      </c>
+      <c r="S48" s="3">
+        <v>0</v>
+      </c>
+      <c r="T48" s="1">
         <v>123</v>
       </c>
-      <c r="R48" s="1">
+      <c r="U48" s="1">
         <v>66</v>
       </c>
-      <c r="S48" s="3">
-        <v>0</v>
-      </c>
-      <c r="T48" s="3">
-        <v>0</v>
-      </c>
-      <c r="U48" s="7"/>
-    </row>
-    <row r="49" spans="1:21" ht="15" customHeight="1" thickBot="1">
+      <c r="V48" s="3">
+        <v>0</v>
+      </c>
+      <c r="W48" s="3">
+        <v>0</v>
+      </c>
+      <c r="X48" s="7"/>
+      <c r="Y48" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z48" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA48" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB48" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC48" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD48" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:30" ht="15" customHeight="1" thickBot="1">
       <c r="A49" s="10" t="s">
         <v>43</v>
       </c>
@@ -5704,21 +7007,48 @@
       <c r="P49" s="3">
         <v>4</v>
       </c>
-      <c r="Q49" s="1">
+      <c r="Q49" s="3">
+        <v>0</v>
+      </c>
+      <c r="R49" s="3">
+        <v>0</v>
+      </c>
+      <c r="S49" s="3">
+        <v>0</v>
+      </c>
+      <c r="T49" s="1">
         <v>119</v>
       </c>
-      <c r="R49" s="1">
+      <c r="U49" s="1">
         <v>102</v>
       </c>
-      <c r="S49" s="3">
-        <v>0</v>
-      </c>
-      <c r="T49" s="3">
-        <v>0</v>
-      </c>
-      <c r="U49" s="7"/>
-    </row>
-    <row r="50" spans="1:21" ht="15" customHeight="1" thickBot="1">
+      <c r="V49" s="3">
+        <v>0</v>
+      </c>
+      <c r="W49" s="3">
+        <v>0</v>
+      </c>
+      <c r="X49" s="7"/>
+      <c r="Y49" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z49" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA49" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB49" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC49" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD49" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:30" ht="15" customHeight="1" thickBot="1">
       <c r="A50" s="10" t="s">
         <v>44</v>
       </c>
@@ -5768,20 +7098,47 @@
         <v>4</v>
       </c>
       <c r="Q50" s="3">
+        <v>0</v>
+      </c>
+      <c r="R50" s="3">
+        <v>0</v>
+      </c>
+      <c r="S50" s="3">
+        <v>0</v>
+      </c>
+      <c r="T50" s="3">
         <v>98</v>
       </c>
-      <c r="R50" s="3">
+      <c r="U50" s="3">
         <v>66</v>
       </c>
-      <c r="S50" s="3">
-        <v>0</v>
-      </c>
-      <c r="T50" s="3">
-        <v>0</v>
-      </c>
-      <c r="U50" s="7"/>
-    </row>
-    <row r="51" spans="1:21" ht="15" customHeight="1" thickTop="1" thickBot="1">
+      <c r="V50" s="3">
+        <v>0</v>
+      </c>
+      <c r="W50" s="3">
+        <v>0</v>
+      </c>
+      <c r="X50" s="7"/>
+      <c r="Y50" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z50" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA50" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB50" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC50" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD50" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:30" ht="15" customHeight="1" thickTop="1" thickBot="1">
       <c r="A51" s="13" t="s">
         <v>45</v>
       </c>
@@ -5831,20 +7188,47 @@
         <v>4</v>
       </c>
       <c r="Q51" s="3">
+        <v>0</v>
+      </c>
+      <c r="R51" s="3">
+        <v>0</v>
+      </c>
+      <c r="S51" s="3">
+        <v>0</v>
+      </c>
+      <c r="T51" s="3">
         <v>98</v>
       </c>
-      <c r="R51" s="3">
+      <c r="U51" s="3">
         <v>66</v>
       </c>
-      <c r="S51" s="3">
-        <v>0</v>
-      </c>
-      <c r="T51" s="3">
-        <v>0</v>
-      </c>
-      <c r="U51" s="7"/>
-    </row>
-    <row r="52" spans="1:21" ht="15" customHeight="1" thickTop="1" thickBot="1">
+      <c r="V51" s="3">
+        <v>0</v>
+      </c>
+      <c r="W51" s="3">
+        <v>0</v>
+      </c>
+      <c r="X51" s="7"/>
+      <c r="Y51" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z51" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA51" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB51" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC51" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD51" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:30" ht="15" customHeight="1" thickTop="1" thickBot="1">
       <c r="A52" s="13" t="s">
         <v>46</v>
       </c>
@@ -5894,20 +7278,47 @@
         <v>4</v>
       </c>
       <c r="Q52" s="3">
+        <v>0</v>
+      </c>
+      <c r="R52" s="3">
+        <v>0</v>
+      </c>
+      <c r="S52" s="3">
+        <v>0</v>
+      </c>
+      <c r="T52" s="3">
         <v>98</v>
       </c>
-      <c r="R52" s="3">
+      <c r="U52" s="3">
         <v>66</v>
       </c>
-      <c r="S52" s="3">
-        <v>0</v>
-      </c>
-      <c r="T52" s="3">
-        <v>0</v>
-      </c>
-      <c r="U52" s="7"/>
-    </row>
-    <row r="53" spans="1:21" ht="15" customHeight="1" thickTop="1" thickBot="1">
+      <c r="V52" s="3">
+        <v>0</v>
+      </c>
+      <c r="W52" s="3">
+        <v>0</v>
+      </c>
+      <c r="X52" s="7"/>
+      <c r="Y52" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z52" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA52" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB52" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC52" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD52" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:30" ht="15" customHeight="1" thickTop="1" thickBot="1">
       <c r="A53" s="13" t="s">
         <v>47</v>
       </c>
@@ -5957,109 +7368,344 @@
         <v>4</v>
       </c>
       <c r="Q53" s="3">
+        <v>0</v>
+      </c>
+      <c r="R53" s="3">
+        <v>0</v>
+      </c>
+      <c r="S53" s="3">
+        <v>0</v>
+      </c>
+      <c r="T53" s="3">
         <v>122</v>
       </c>
-      <c r="R53" s="3">
+      <c r="U53" s="3">
         <v>74</v>
       </c>
-      <c r="S53" s="3">
-        <v>0</v>
-      </c>
-      <c r="T53" s="3">
-        <v>0</v>
-      </c>
-      <c r="U53" s="7"/>
-    </row>
-    <row r="54" spans="1:21" ht="15" customHeight="1" thickTop="1" thickBot="1">
+      <c r="V53" s="3">
+        <v>0</v>
+      </c>
+      <c r="W53" s="3">
+        <v>0</v>
+      </c>
+      <c r="X53" s="7"/>
+      <c r="Y53" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z53" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA53" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB53" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC53" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD53" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:30" ht="15" customHeight="1" thickTop="1" thickBot="1">
       <c r="A54" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B54" s="3">
+        <v>0</v>
+      </c>
+      <c r="C54" s="3">
+        <v>0</v>
+      </c>
+      <c r="D54" s="3">
+        <v>0</v>
+      </c>
+      <c r="E54" s="3">
+        <v>0</v>
+      </c>
+      <c r="F54" s="3">
+        <v>0</v>
+      </c>
+      <c r="G54" s="3">
+        <v>0</v>
+      </c>
+      <c r="H54" s="3">
+        <v>0</v>
+      </c>
+      <c r="I54" s="3">
+        <v>0</v>
+      </c>
+      <c r="J54" s="3">
+        <v>0</v>
+      </c>
+      <c r="K54" s="3">
+        <v>0</v>
+      </c>
+      <c r="L54" s="3">
+        <v>0</v>
+      </c>
+      <c r="M54" s="3">
+        <v>0</v>
+      </c>
+      <c r="N54" s="3">
+        <v>0</v>
+      </c>
+      <c r="O54" s="3">
+        <v>0</v>
+      </c>
+      <c r="P54" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q54" s="3">
+        <v>0</v>
+      </c>
+      <c r="R54" s="3">
+        <v>0</v>
+      </c>
+      <c r="S54" s="3">
+        <v>0</v>
+      </c>
+      <c r="T54" s="3">
+        <v>0</v>
+      </c>
+      <c r="U54" s="3">
+        <v>0</v>
+      </c>
+      <c r="V54" s="3">
+        <v>0</v>
+      </c>
+      <c r="W54" s="3">
+        <v>0</v>
+      </c>
+      <c r="X54" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y54" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z54" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA54" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB54" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC54" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD54" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:30" ht="15" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A55" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="B54" s="3">
+      <c r="B55" s="3">
         <v>5</v>
       </c>
-      <c r="C54" s="3">
+      <c r="C55" s="3">
         <v>16</v>
       </c>
-      <c r="D54" s="3">
-        <v>0</v>
-      </c>
-      <c r="E54" s="3">
-        <v>0</v>
-      </c>
-      <c r="F54" s="3">
-        <v>0</v>
-      </c>
-      <c r="G54" s="3">
-        <v>0</v>
-      </c>
-      <c r="H54" s="3">
-        <v>0</v>
-      </c>
-      <c r="I54" s="3">
-        <v>0</v>
-      </c>
-      <c r="J54" s="3">
-        <v>0</v>
-      </c>
-      <c r="K54" s="3">
-        <v>0</v>
-      </c>
-      <c r="L54" s="3">
+      <c r="D55" s="3">
+        <v>0</v>
+      </c>
+      <c r="E55" s="3">
+        <v>0</v>
+      </c>
+      <c r="F55" s="3">
+        <v>0</v>
+      </c>
+      <c r="G55" s="3">
+        <v>0</v>
+      </c>
+      <c r="H55" s="3">
+        <v>0</v>
+      </c>
+      <c r="I55" s="3">
+        <v>0</v>
+      </c>
+      <c r="J55" s="3">
+        <v>0</v>
+      </c>
+      <c r="K55" s="3">
+        <v>0</v>
+      </c>
+      <c r="L55" s="3">
         <v>2</v>
       </c>
-      <c r="M54" s="3">
+      <c r="M55" s="3">
         <v>2</v>
       </c>
-      <c r="N54" s="3">
-        <v>0</v>
-      </c>
-      <c r="O54" s="3">
-        <v>0</v>
-      </c>
-      <c r="P54" s="3">
+      <c r="N55" s="3">
+        <v>0</v>
+      </c>
+      <c r="O55" s="3">
+        <v>0</v>
+      </c>
+      <c r="P55" s="3">
         <v>1</v>
       </c>
-      <c r="Q54" s="3">
+      <c r="Q55" s="3">
+        <v>0</v>
+      </c>
+      <c r="R55" s="3">
+        <v>0</v>
+      </c>
+      <c r="S55" s="3">
+        <v>0</v>
+      </c>
+      <c r="T55" s="3">
         <v>10</v>
       </c>
-      <c r="R54" s="3">
+      <c r="U55" s="3">
         <v>6</v>
       </c>
-      <c r="S54" s="3">
-        <v>0</v>
-      </c>
-      <c r="T54" s="3">
-        <v>0</v>
-      </c>
-      <c r="U54" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:21" ht="15" customHeight="1">
-      <c r="A56" s="21"/>
-    </row>
-    <row r="57" spans="1:21" ht="15" customHeight="1">
-      <c r="A57" s="20"/>
-    </row>
-    <row r="58" spans="1:21" ht="15" customHeight="1">
+      <c r="V55" s="3">
+        <v>0</v>
+      </c>
+      <c r="W55" s="3">
+        <v>0</v>
+      </c>
+      <c r="X55" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y55" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z55" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA55" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB55" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC55" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD55" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:30" ht="15" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A56" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B56" s="3">
+        <v>0</v>
+      </c>
+      <c r="C56" s="3">
+        <v>0</v>
+      </c>
+      <c r="D56" s="3">
+        <v>0</v>
+      </c>
+      <c r="E56" s="3">
+        <v>0</v>
+      </c>
+      <c r="F56" s="3">
+        <v>0</v>
+      </c>
+      <c r="G56" s="3">
+        <v>0</v>
+      </c>
+      <c r="H56" s="3">
+        <v>0</v>
+      </c>
+      <c r="I56" s="3">
+        <v>0</v>
+      </c>
+      <c r="J56" s="3">
+        <v>0</v>
+      </c>
+      <c r="K56" s="3">
+        <v>0</v>
+      </c>
+      <c r="L56" s="3">
+        <v>0</v>
+      </c>
+      <c r="M56" s="3">
+        <v>0</v>
+      </c>
+      <c r="N56" s="3">
+        <v>0</v>
+      </c>
+      <c r="O56" s="3">
+        <v>0</v>
+      </c>
+      <c r="P56" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q56" s="3">
+        <v>0</v>
+      </c>
+      <c r="R56" s="3">
+        <v>0</v>
+      </c>
+      <c r="S56" s="3">
+        <v>0</v>
+      </c>
+      <c r="T56" s="3">
+        <v>0</v>
+      </c>
+      <c r="U56" s="3">
+        <v>0</v>
+      </c>
+      <c r="V56" s="3">
+        <v>0</v>
+      </c>
+      <c r="W56" s="3">
+        <v>0</v>
+      </c>
+      <c r="X56" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y56" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z56" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA56" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB56" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC56" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD56" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:30" ht="15" customHeight="1">
+      <c r="A57" s="21"/>
+    </row>
+    <row r="58" spans="1:30" ht="15" customHeight="1">
       <c r="A58" s="20"/>
     </row>
-    <row r="59" spans="1:21" ht="15" customHeight="1">
+    <row r="59" spans="1:30" ht="15" customHeight="1">
       <c r="A59" s="20"/>
     </row>
-    <row r="60" spans="1:21" ht="15" customHeight="1">
+    <row r="60" spans="1:30" ht="15" customHeight="1">
       <c r="A60" s="20"/>
     </row>
-    <row r="61" spans="1:21" ht="15" customHeight="1">
+    <row r="61" spans="1:30" ht="15" customHeight="1">
       <c r="A61" s="20"/>
     </row>
-    <row r="62" spans="1:21" ht="15" customHeight="1">
+    <row r="62" spans="1:30" ht="15" customHeight="1">
       <c r="A62" s="20"/>
     </row>
-    <row r="63" spans="1:21" ht="15" customHeight="1">
+    <row r="63" spans="1:30" ht="15" customHeight="1">
       <c r="A63" s="20"/>
     </row>
-    <row r="64" spans="1:21" ht="15" customHeight="1">
+    <row r="64" spans="1:30" ht="15" customHeight="1">
       <c r="A64" s="20"/>
     </row>
     <row r="65" spans="1:1" ht="15" customHeight="1">
@@ -6114,7 +7760,7 @@
       <c r="A81" s="20"/>
     </row>
     <row r="82" spans="1:1" ht="15" customHeight="1">
-      <c r="A82" s="19"/>
+      <c r="A82" s="20"/>
     </row>
     <row r="83" spans="1:1" ht="15" customHeight="1">
       <c r="A83" s="19"/>
@@ -6256,6 +7902,9 @@
     </row>
     <row r="129" spans="1:1" ht="15" customHeight="1">
       <c r="A129" s="19"/>
+    </row>
+    <row r="130" spans="1:1" ht="15" customHeight="1">
+      <c r="A130" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.35433070866141736" bottom="0.35433070866141736" header="0" footer="0"/>

</xml_diff>

<commit_message>
Add: sixth ipr seeder
</commit_message>
<xml_diff>
--- a/storage/app/iprs/1/iprs.xlsx
+++ b/storage/app/iprs/1/iprs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Smoku\Pfron\pfron-backend\storage\app\iprs\1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B160D71-5400-457F-9A00-D1D1E8552C4B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC1E5228-C61D-4BA1-99BE-D9E2C45A4636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t>id</t>
   </si>
@@ -189,6 +189,27 @@
   <si>
     <t>M1-W055</t>
   </si>
+  <si>
+    <t>M1-W056</t>
+  </si>
+  <si>
+    <t>M1-W057</t>
+  </si>
+  <si>
+    <t>M1-W058</t>
+  </si>
+  <si>
+    <t>M1-W059</t>
+  </si>
+  <si>
+    <t>M1-W060</t>
+  </si>
+  <si>
+    <t>M1-W061</t>
+  </si>
+  <si>
+    <t>M1-W062</t>
+  </si>
 </sst>
 </file>
 
@@ -840,13 +861,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="238"/>
-      <scheme val="minor"/>
+      <sz val="8"/>
+      <name val="Czcionka tekstu podstawowego"/>
     </font>
   </fonts>
   <fills count="49">
@@ -1130,7 +1146,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -1437,6 +1453,17 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -1947,9 +1974,6 @@
     </xf>
     <xf numFmtId="0" fontId="86" fillId="47" borderId="0" xfId="261" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="86" fillId="48" borderId="0" xfId="261" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="87" fillId="0" borderId="0" xfId="261" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="86" fillId="4" borderId="23" xfId="261" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1958,6 +1982,9 @@
     </xf>
     <xf numFmtId="0" fontId="86" fillId="46" borderId="23" xfId="261" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="423">
@@ -2602,10 +2629,10 @@
   <dimension ref="A1:AD130"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="O29" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="O35" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A56" sqref="A56"/>
+      <selection pane="bottomRight" activeCell="AB52" sqref="AB52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
@@ -4608,49 +4635,49 @@
       <c r="A23" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="B23" s="22">
+      <c r="B23" s="21">
         <v>12</v>
       </c>
-      <c r="C23" s="22">
+      <c r="C23" s="21">
         <v>40</v>
       </c>
-      <c r="D23" s="22">
+      <c r="D23" s="21">
         <v>25</v>
       </c>
-      <c r="E23" s="22">
+      <c r="E23" s="21">
         <v>80</v>
       </c>
-      <c r="F23" s="22">
+      <c r="F23" s="21">
         <v>227</v>
       </c>
-      <c r="G23" s="22">
-        <v>0</v>
-      </c>
-      <c r="H23" s="22">
+      <c r="G23" s="21">
+        <v>0</v>
+      </c>
+      <c r="H23" s="21">
         <v>11</v>
       </c>
-      <c r="I23" s="22">
-        <v>0</v>
-      </c>
-      <c r="J23" s="22">
-        <v>0</v>
-      </c>
-      <c r="K23" s="22">
-        <v>0</v>
-      </c>
-      <c r="L23" s="23">
+      <c r="I23" s="21">
+        <v>0</v>
+      </c>
+      <c r="J23" s="21">
+        <v>0</v>
+      </c>
+      <c r="K23" s="21">
+        <v>0</v>
+      </c>
+      <c r="L23" s="22">
         <v>7</v>
       </c>
-      <c r="M23" s="22">
+      <c r="M23" s="21">
         <v>39</v>
       </c>
-      <c r="N23" s="22">
+      <c r="N23" s="21">
         <v>2</v>
       </c>
-      <c r="O23" s="22">
+      <c r="O23" s="21">
         <v>1</v>
       </c>
-      <c r="P23" s="22">
+      <c r="P23" s="21">
         <v>4</v>
       </c>
       <c r="Q23" s="3">
@@ -4662,19 +4689,19 @@
       <c r="S23" s="3">
         <v>0</v>
       </c>
-      <c r="T23" s="22">
+      <c r="T23" s="21">
         <v>130</v>
       </c>
-      <c r="U23" s="22">
+      <c r="U23" s="21">
         <v>82</v>
       </c>
-      <c r="V23" s="22">
+      <c r="V23" s="21">
         <v>3</v>
       </c>
-      <c r="W23" s="22">
+      <c r="W23" s="21">
         <v>2</v>
       </c>
-      <c r="X23" s="24"/>
+      <c r="X23" s="23"/>
       <c r="Y23" s="3">
         <v>0</v>
       </c>
@@ -7684,26 +7711,649 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:30" ht="15" customHeight="1">
-      <c r="A57" s="21"/>
-    </row>
-    <row r="58" spans="1:30" ht="15" customHeight="1">
-      <c r="A58" s="20"/>
-    </row>
-    <row r="59" spans="1:30" ht="15" customHeight="1">
-      <c r="A59" s="20"/>
-    </row>
-    <row r="60" spans="1:30" ht="15" customHeight="1">
-      <c r="A60" s="20"/>
-    </row>
-    <row r="61" spans="1:30" ht="15" customHeight="1">
-      <c r="A61" s="20"/>
-    </row>
-    <row r="62" spans="1:30" ht="15" customHeight="1">
-      <c r="A62" s="20"/>
-    </row>
-    <row r="63" spans="1:30" ht="15" customHeight="1">
-      <c r="A63" s="20"/>
+    <row r="57" spans="1:30" ht="15" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A57" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B57" s="24">
+        <v>0</v>
+      </c>
+      <c r="C57" s="24">
+        <v>0</v>
+      </c>
+      <c r="D57" s="24">
+        <v>0</v>
+      </c>
+      <c r="E57" s="24">
+        <v>0</v>
+      </c>
+      <c r="F57" s="24">
+        <v>0</v>
+      </c>
+      <c r="G57" s="24">
+        <v>0</v>
+      </c>
+      <c r="H57" s="24">
+        <v>0</v>
+      </c>
+      <c r="I57" s="24">
+        <v>0</v>
+      </c>
+      <c r="J57" s="24">
+        <v>0</v>
+      </c>
+      <c r="K57" s="24">
+        <v>0</v>
+      </c>
+      <c r="L57" s="24">
+        <v>0</v>
+      </c>
+      <c r="M57" s="24">
+        <v>0</v>
+      </c>
+      <c r="N57" s="24">
+        <v>0</v>
+      </c>
+      <c r="O57" s="24">
+        <v>0</v>
+      </c>
+      <c r="P57" s="24">
+        <v>0</v>
+      </c>
+      <c r="Q57" s="24">
+        <v>0</v>
+      </c>
+      <c r="R57" s="24">
+        <v>0</v>
+      </c>
+      <c r="S57" s="24">
+        <v>0</v>
+      </c>
+      <c r="T57" s="24">
+        <v>0</v>
+      </c>
+      <c r="U57" s="24">
+        <v>0</v>
+      </c>
+      <c r="V57" s="24">
+        <v>0</v>
+      </c>
+      <c r="W57" s="24">
+        <v>0</v>
+      </c>
+      <c r="X57" s="24">
+        <v>0</v>
+      </c>
+      <c r="Y57" s="24">
+        <v>0</v>
+      </c>
+      <c r="Z57" s="24">
+        <v>0</v>
+      </c>
+      <c r="AA57" s="24">
+        <v>0</v>
+      </c>
+      <c r="AB57" s="24">
+        <v>0</v>
+      </c>
+      <c r="AC57" s="24">
+        <v>0</v>
+      </c>
+      <c r="AD57" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:30" ht="15" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A58" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B58" s="24">
+        <v>0</v>
+      </c>
+      <c r="C58" s="24">
+        <v>0</v>
+      </c>
+      <c r="D58" s="24">
+        <v>0</v>
+      </c>
+      <c r="E58" s="24">
+        <v>0</v>
+      </c>
+      <c r="F58" s="24">
+        <v>0</v>
+      </c>
+      <c r="G58" s="24">
+        <v>0</v>
+      </c>
+      <c r="H58" s="24">
+        <v>0</v>
+      </c>
+      <c r="I58" s="24">
+        <v>0</v>
+      </c>
+      <c r="J58" s="24">
+        <v>0</v>
+      </c>
+      <c r="K58" s="24">
+        <v>0</v>
+      </c>
+      <c r="L58" s="24">
+        <v>0</v>
+      </c>
+      <c r="M58" s="24">
+        <v>0</v>
+      </c>
+      <c r="N58" s="24">
+        <v>0</v>
+      </c>
+      <c r="O58" s="24">
+        <v>0</v>
+      </c>
+      <c r="P58" s="24">
+        <v>0</v>
+      </c>
+      <c r="Q58" s="24">
+        <v>0</v>
+      </c>
+      <c r="R58" s="24">
+        <v>0</v>
+      </c>
+      <c r="S58" s="24">
+        <v>0</v>
+      </c>
+      <c r="T58" s="24">
+        <v>0</v>
+      </c>
+      <c r="U58" s="24">
+        <v>0</v>
+      </c>
+      <c r="V58" s="24">
+        <v>0</v>
+      </c>
+      <c r="W58" s="24">
+        <v>0</v>
+      </c>
+      <c r="X58" s="24">
+        <v>0</v>
+      </c>
+      <c r="Y58" s="24">
+        <v>0</v>
+      </c>
+      <c r="Z58" s="24">
+        <v>0</v>
+      </c>
+      <c r="AA58" s="24">
+        <v>0</v>
+      </c>
+      <c r="AB58" s="24">
+        <v>0</v>
+      </c>
+      <c r="AC58" s="24">
+        <v>0</v>
+      </c>
+      <c r="AD58" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:30" ht="15" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A59" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B59" s="24">
+        <v>0</v>
+      </c>
+      <c r="C59" s="24">
+        <v>0</v>
+      </c>
+      <c r="D59" s="24">
+        <v>0</v>
+      </c>
+      <c r="E59" s="24">
+        <v>0</v>
+      </c>
+      <c r="F59" s="24">
+        <v>0</v>
+      </c>
+      <c r="G59" s="24">
+        <v>0</v>
+      </c>
+      <c r="H59" s="24">
+        <v>0</v>
+      </c>
+      <c r="I59" s="24">
+        <v>0</v>
+      </c>
+      <c r="J59" s="24">
+        <v>0</v>
+      </c>
+      <c r="K59" s="24">
+        <v>0</v>
+      </c>
+      <c r="L59" s="24">
+        <v>0</v>
+      </c>
+      <c r="M59" s="24">
+        <v>0</v>
+      </c>
+      <c r="N59" s="24">
+        <v>0</v>
+      </c>
+      <c r="O59" s="24">
+        <v>0</v>
+      </c>
+      <c r="P59" s="24">
+        <v>0</v>
+      </c>
+      <c r="Q59" s="24">
+        <v>0</v>
+      </c>
+      <c r="R59" s="24">
+        <v>0</v>
+      </c>
+      <c r="S59" s="24">
+        <v>0</v>
+      </c>
+      <c r="T59" s="24">
+        <v>0</v>
+      </c>
+      <c r="U59" s="24">
+        <v>0</v>
+      </c>
+      <c r="V59" s="24">
+        <v>0</v>
+      </c>
+      <c r="W59" s="24">
+        <v>0</v>
+      </c>
+      <c r="X59" s="24">
+        <v>0</v>
+      </c>
+      <c r="Y59" s="24">
+        <v>0</v>
+      </c>
+      <c r="Z59" s="24">
+        <v>0</v>
+      </c>
+      <c r="AA59" s="24">
+        <v>0</v>
+      </c>
+      <c r="AB59" s="24">
+        <v>0</v>
+      </c>
+      <c r="AC59" s="24">
+        <v>0</v>
+      </c>
+      <c r="AD59" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:30" ht="15" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A60" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B60" s="24">
+        <v>0</v>
+      </c>
+      <c r="C60" s="24">
+        <v>0</v>
+      </c>
+      <c r="D60" s="24">
+        <v>0</v>
+      </c>
+      <c r="E60" s="24">
+        <v>0</v>
+      </c>
+      <c r="F60" s="24">
+        <v>0</v>
+      </c>
+      <c r="G60" s="24">
+        <v>0</v>
+      </c>
+      <c r="H60" s="24">
+        <v>0</v>
+      </c>
+      <c r="I60" s="24">
+        <v>0</v>
+      </c>
+      <c r="J60" s="24">
+        <v>0</v>
+      </c>
+      <c r="K60" s="24">
+        <v>0</v>
+      </c>
+      <c r="L60" s="24">
+        <v>0</v>
+      </c>
+      <c r="M60" s="24">
+        <v>0</v>
+      </c>
+      <c r="N60" s="24">
+        <v>0</v>
+      </c>
+      <c r="O60" s="24">
+        <v>0</v>
+      </c>
+      <c r="P60" s="24">
+        <v>0</v>
+      </c>
+      <c r="Q60" s="24">
+        <v>0</v>
+      </c>
+      <c r="R60" s="24">
+        <v>0</v>
+      </c>
+      <c r="S60" s="24">
+        <v>0</v>
+      </c>
+      <c r="T60" s="24">
+        <v>0</v>
+      </c>
+      <c r="U60" s="24">
+        <v>0</v>
+      </c>
+      <c r="V60" s="24">
+        <v>0</v>
+      </c>
+      <c r="W60" s="24">
+        <v>0</v>
+      </c>
+      <c r="X60" s="24">
+        <v>0</v>
+      </c>
+      <c r="Y60" s="24">
+        <v>0</v>
+      </c>
+      <c r="Z60" s="24">
+        <v>0</v>
+      </c>
+      <c r="AA60" s="24">
+        <v>0</v>
+      </c>
+      <c r="AB60" s="24">
+        <v>0</v>
+      </c>
+      <c r="AC60" s="24">
+        <v>0</v>
+      </c>
+      <c r="AD60" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:30" ht="15" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A61" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="B61" s="24">
+        <v>0</v>
+      </c>
+      <c r="C61" s="24">
+        <v>0</v>
+      </c>
+      <c r="D61" s="24">
+        <v>0</v>
+      </c>
+      <c r="E61" s="24">
+        <v>0</v>
+      </c>
+      <c r="F61" s="24">
+        <v>0</v>
+      </c>
+      <c r="G61" s="24">
+        <v>0</v>
+      </c>
+      <c r="H61" s="24">
+        <v>0</v>
+      </c>
+      <c r="I61" s="24">
+        <v>0</v>
+      </c>
+      <c r="J61" s="24">
+        <v>0</v>
+      </c>
+      <c r="K61" s="24">
+        <v>0</v>
+      </c>
+      <c r="L61" s="24">
+        <v>0</v>
+      </c>
+      <c r="M61" s="24">
+        <v>0</v>
+      </c>
+      <c r="N61" s="24">
+        <v>0</v>
+      </c>
+      <c r="O61" s="24">
+        <v>0</v>
+      </c>
+      <c r="P61" s="24">
+        <v>0</v>
+      </c>
+      <c r="Q61" s="24">
+        <v>0</v>
+      </c>
+      <c r="R61" s="24">
+        <v>0</v>
+      </c>
+      <c r="S61" s="24">
+        <v>0</v>
+      </c>
+      <c r="T61" s="24">
+        <v>0</v>
+      </c>
+      <c r="U61" s="24">
+        <v>0</v>
+      </c>
+      <c r="V61" s="24">
+        <v>0</v>
+      </c>
+      <c r="W61" s="24">
+        <v>0</v>
+      </c>
+      <c r="X61" s="24">
+        <v>0</v>
+      </c>
+      <c r="Y61" s="24">
+        <v>0</v>
+      </c>
+      <c r="Z61" s="24">
+        <v>0</v>
+      </c>
+      <c r="AA61" s="24">
+        <v>0</v>
+      </c>
+      <c r="AB61" s="24">
+        <v>0</v>
+      </c>
+      <c r="AC61" s="24">
+        <v>0</v>
+      </c>
+      <c r="AD61" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:30" ht="15" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A62" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="B62" s="24">
+        <v>0</v>
+      </c>
+      <c r="C62" s="24">
+        <v>0</v>
+      </c>
+      <c r="D62" s="24">
+        <v>0</v>
+      </c>
+      <c r="E62" s="24">
+        <v>0</v>
+      </c>
+      <c r="F62" s="24">
+        <v>0</v>
+      </c>
+      <c r="G62" s="24">
+        <v>0</v>
+      </c>
+      <c r="H62" s="24">
+        <v>0</v>
+      </c>
+      <c r="I62" s="24">
+        <v>0</v>
+      </c>
+      <c r="J62" s="24">
+        <v>0</v>
+      </c>
+      <c r="K62" s="24">
+        <v>0</v>
+      </c>
+      <c r="L62" s="24">
+        <v>0</v>
+      </c>
+      <c r="M62" s="24">
+        <v>0</v>
+      </c>
+      <c r="N62" s="24">
+        <v>0</v>
+      </c>
+      <c r="O62" s="24">
+        <v>0</v>
+      </c>
+      <c r="P62" s="24">
+        <v>0</v>
+      </c>
+      <c r="Q62" s="24">
+        <v>0</v>
+      </c>
+      <c r="R62" s="24">
+        <v>0</v>
+      </c>
+      <c r="S62" s="24">
+        <v>0</v>
+      </c>
+      <c r="T62" s="24">
+        <v>0</v>
+      </c>
+      <c r="U62" s="24">
+        <v>0</v>
+      </c>
+      <c r="V62" s="24">
+        <v>0</v>
+      </c>
+      <c r="W62" s="24">
+        <v>0</v>
+      </c>
+      <c r="X62" s="24">
+        <v>0</v>
+      </c>
+      <c r="Y62" s="24">
+        <v>0</v>
+      </c>
+      <c r="Z62" s="24">
+        <v>0</v>
+      </c>
+      <c r="AA62" s="24">
+        <v>0</v>
+      </c>
+      <c r="AB62" s="24">
+        <v>0</v>
+      </c>
+      <c r="AC62" s="24">
+        <v>0</v>
+      </c>
+      <c r="AD62" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:30" ht="15" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A63" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="B63" s="24">
+        <v>0</v>
+      </c>
+      <c r="C63" s="24">
+        <v>0</v>
+      </c>
+      <c r="D63" s="24">
+        <v>0</v>
+      </c>
+      <c r="E63" s="24">
+        <v>0</v>
+      </c>
+      <c r="F63" s="24">
+        <v>0</v>
+      </c>
+      <c r="G63" s="24">
+        <v>0</v>
+      </c>
+      <c r="H63" s="24">
+        <v>0</v>
+      </c>
+      <c r="I63" s="24">
+        <v>0</v>
+      </c>
+      <c r="J63" s="24">
+        <v>0</v>
+      </c>
+      <c r="K63" s="24">
+        <v>0</v>
+      </c>
+      <c r="L63" s="24">
+        <v>0</v>
+      </c>
+      <c r="M63" s="24">
+        <v>0</v>
+      </c>
+      <c r="N63" s="24">
+        <v>0</v>
+      </c>
+      <c r="O63" s="24">
+        <v>0</v>
+      </c>
+      <c r="P63" s="24">
+        <v>0</v>
+      </c>
+      <c r="Q63" s="24">
+        <v>0</v>
+      </c>
+      <c r="R63" s="24">
+        <v>0</v>
+      </c>
+      <c r="S63" s="24">
+        <v>0</v>
+      </c>
+      <c r="T63" s="24">
+        <v>0</v>
+      </c>
+      <c r="U63" s="24">
+        <v>0</v>
+      </c>
+      <c r="V63" s="24">
+        <v>0</v>
+      </c>
+      <c r="W63" s="24">
+        <v>0</v>
+      </c>
+      <c r="X63" s="24">
+        <v>0</v>
+      </c>
+      <c r="Y63" s="24">
+        <v>0</v>
+      </c>
+      <c r="Z63" s="24">
+        <v>0</v>
+      </c>
+      <c r="AA63" s="24">
+        <v>0</v>
+      </c>
+      <c r="AB63" s="24">
+        <v>0</v>
+      </c>
+      <c r="AC63" s="24">
+        <v>0</v>
+      </c>
+      <c r="AD63" s="24">
+        <v>0</v>
+      </c>
     </row>
     <row r="64" spans="1:30" ht="15" customHeight="1">
       <c r="A64" s="20"/>
@@ -7907,6 +8557,7 @@
       <c r="A130" s="19"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="87" type="noConversion"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.35433070866141736" bottom="0.35433070866141736" header="0" footer="0"/>
   <pageSetup paperSize="9" fitToWidth="0" orientation="landscape" r:id="rId1"/>
 </worksheet>

</xml_diff>